<commit_message>
start on report writing
</commit_message>
<xml_diff>
--- a/Group Registration.xlsx
+++ b/Group Registration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0424632_u_nus_edu/Documents/Academics/TA/IS4242/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericdrake/Desktop/NUS/IS4242/Group/LLP_IS4242/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{289DE5C5-817E-4A8A-B288-63F78D2D0948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64FC0760-0657-486E-98B5-EF2E59B99DE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE3F621-6962-2947-B206-EF1BDBDE5660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{AC476BA7-6860-4039-A242-F6B6BCCB68AF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19600" xr2:uid="{AC476BA7-6860-4039-A242-F6B6BCCB68AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Group Registration" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Student Name</t>
   </si>
@@ -41,31 +41,68 @@
   </si>
   <si>
     <t>Group Name</t>
+  </si>
+  <si>
+    <t>Haocheng Lu</t>
+  </si>
+  <si>
+    <t>A0276434Y</t>
+  </si>
+  <si>
+    <t>LLP</t>
+  </si>
+  <si>
+    <t>Paul David Christopher Golling</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0294203L</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>LUO Ming</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0244396W</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>E1132167</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>E1345974</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>E0860682</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -73,7 +110,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -81,7 +118,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -89,35 +126,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -125,7 +162,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -133,14 +170,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -148,14 +185,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -163,7 +200,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -171,15 +208,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -524,53 +575,54 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,7 +638,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -905,19 +957,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="U16" sqref="T15:U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,22 +983,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>